<commit_message>
Fixed spelling and new excel doc
</commit_message>
<xml_diff>
--- a/public/assets/Lokalbokning template.xlsx
+++ b/public/assets/Lokalbokning template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>Lokal</t>
   </si>
@@ -97,7 +97,7 @@
     <t>2030-01-01 17:00</t>
   </si>
   <si>
-    <t>Exportera som .csv</t>
+    <t>Gör så här:</t>
   </si>
   <si>
     <t>Focus studiedel</t>
@@ -121,6 +121,9 @@
     <t>Nekad</t>
   </si>
   <si>
+    <t>1. Infoga en rad för varje bokning du vill göra</t>
+  </si>
+  <si>
     <t>Föreställning</t>
   </si>
   <si>
@@ -139,7 +142,7 @@
     <t>Godkänd</t>
   </si>
   <si>
-    <t>Från, Till och Stående till måste anges i samma format som i exemplet. (Tiden antas vara relativ stockholms tidszon)</t>
+    <t>2. Exportera som .csv när du är klar</t>
   </si>
   <si>
     <t>Övrig bokning</t>
@@ -154,14 +157,128 @@
     <t>2025-07-02 03:00</t>
   </si>
   <si>
-    <t>Stående bokning måste vara exakt som i exemplet (stava inte fel)</t>
+    <t>OBS:</t>
+  </si>
+  <si>
+    <t>Ändra INTE namn på kolumnerna (alltså rad 1)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Från</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Till</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> och </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Stående till</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> måste anges i samma format som i exemplet. (Tiden antas vara relativ stockholms tidszon)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Lokal, Typ, Stående bokning </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>och</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Status </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>måste vara exakt som i exemplet (stava inte fel)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Stående till</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> får bara vara tom om</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Stående bokning</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> är 'Aldrig'</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -179,8 +296,15 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +315,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
         <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -218,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -231,6 +361,15 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -580,7 +719,7 @@
         <v>20</v>
       </c>
       <c r="L3" s="5"/>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="6" t="s">
         <v>28</v>
       </c>
     </row>
@@ -619,6 +758,9 @@
         <v>35</v>
       </c>
       <c r="L4" s="5"/>
+      <c r="M4" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
@@ -634,29 +776,29 @@
         <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -673,43 +815,55 @@
         <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L6" s="5"/>
-      <c r="M6" s="4" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="7">
       <c r="L7" s="5"/>
+      <c r="M7" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8">
       <c r="L8" s="5"/>
+      <c r="M8" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="9">
       <c r="L9" s="5"/>
+      <c r="M9" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10">
       <c r="L10" s="5"/>
+      <c r="M10" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11">
       <c r="L11" s="5"/>
+      <c r="M11" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12">
       <c r="L12" s="5"/>

</xml_diff>